<commit_message>
Create excel sales list
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinii\OneDrive\Documentos\UiPath\NubankRpaCase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CF3F6E-C77B-48B7-BE1C-3C69F89D0FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C57CD2-8F49-440A-8E8D-EA5C6CCD7410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27720" yWindow="1080" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -165,7 +165,13 @@
     <t>ExcelColumnsToBeAdded</t>
   </si>
   <si>
-    <t>Valor Unitário (BRL), Valor Total (BRL), Data/Hora, Conversão do Câmbio, Endereço, Bairro, Localidade/UF, Erros Encontrados</t>
+    <t>Valor Unitário (BRL), Valor Total (BRL), Data/Hora Conversão do Câmbio, Endereço, Bairro, Localidade/UF, Erros Encontrados</t>
+  </si>
+  <si>
+    <t>Url_PostalCodeSearch</t>
+  </si>
+  <si>
+    <t>Url_PostalCode</t>
   </si>
 </sst>
 </file>
@@ -543,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1626,7 +1632,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2795,7 +2801,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2841,7 +2849,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
create sequence to fill template
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinii\OneDrive\Documentos\UiPath\NubankRpaCase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5B1F88-3780-4167-9FDB-88641C610340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C3A27F-848E-4C0E-9DB1-7C74A7D25358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7665" yWindow="1815" windowWidth="13605" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -166,12 +166,6 @@
   </si>
   <si>
     <t>Valor Unitário (BRL), Valor Total (BRL), Data/Hora Conversão do Câmbio, Endereço, Bairro, Localidade/UF, Erros Encontrados</t>
-  </si>
-  <si>
-    <t>Url_PostalCodeSearch</t>
-  </si>
-  <si>
-    <t>Url_PostalCode</t>
   </si>
   <si>
     <t>EmailReport</t>
@@ -195,12 +189,18 @@
 &lt;/body&gt;
 &lt;/html&gt;</t>
   </si>
+  <si>
+    <t>Url_Quote</t>
+  </si>
+  <si>
+    <t>Url_CEP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -230,6 +230,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -251,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -267,6 +272,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1665,7 +1671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1857,18 +1863,18 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2856,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2906,21 +2912,28 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
+      <c r="A3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>